<commit_message>
updated MPM & Pflichtenheft
</commit_message>
<xml_diff>
--- a/Projektmanagement/Projektstrukturplan.xlsx
+++ b/Projektmanagement/Projektstrukturplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hmedu-my.sharepoint.com/personal/linus_englert_hm_edu/Documents/SoSe2023/Software_Engineering_II/SE_Studienarbeit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="785" documentId="11_AD4DB114E441178AC67DF4E9AE56C532693EDF27" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B48B457E-31A1-4405-B333-2F909CB61330}"/>
+  <xr:revisionPtr revIDLastSave="787" documentId="11_AD4DB114E441178AC67DF4E9AE56C532693EDF27" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D83DB558-D873-4545-AD34-F4EFDE884F7D}"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="160" windowWidth="19100" windowHeight="20800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="210" yWindow="80" windowWidth="19100" windowHeight="20800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektstrukturplan" sheetId="1" r:id="rId1"/>
@@ -1278,7 +1278,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1288,6 +1288,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1304,10 +1310,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1316,18 +1335,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1344,6 +1351,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1637,7 +1648,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1655,452 +1666,452 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3" t="s">
+      <c r="H1" s="8"/>
+      <c r="I1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="9" t="s">
+      <c r="F2" s="9"/>
+      <c r="G2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9" t="s">
+      <c r="H2" s="7"/>
+      <c r="I2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="9"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="4" t="s">
+      <c r="B3" s="9"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="7" t="s">
+      <c r="F3" s="9"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="I3" s="6"/>
-      <c r="J3" s="7" t="s">
+      <c r="I3" s="3"/>
+      <c r="J3" s="4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="4" t="s">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7" t="s">
+      <c r="F4" s="9"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="7" t="s">
+      <c r="I4" s="2"/>
+      <c r="J4" s="4" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="9" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="9"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="7" t="s">
+      <c r="H5" s="7"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="4" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6" t="s">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="7" t="s">
+      <c r="I6" s="3"/>
+      <c r="J6" s="4" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="7" t="s">
+      <c r="I7" s="3"/>
+      <c r="J7" s="4" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="9" t="s">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="9"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="7" t="s">
+      <c r="H8" s="7"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="4" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="7" t="s">
+      <c r="I9" s="3"/>
+      <c r="J9" s="4" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="J10" s="9"/>
+      <c r="J10" s="7"/>
     </row>
     <row r="11" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="9" t="s">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="9"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="6" t="s">
+      <c r="H11" s="7"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="3" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="29" x14ac:dyDescent="0.35">
-      <c r="A12" s="6"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6" t="s">
+      <c r="I12" s="3"/>
+      <c r="J12" s="3" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6" t="s">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6" t="s">
+      <c r="I13" s="3"/>
+      <c r="J13" s="3" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="9" t="s">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J14" s="9"/>
+      <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="7" t="s">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="4" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6" t="s">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="9" t="s">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="J18" s="9"/>
+      <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6" t="s">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6" t="s">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6" t="s">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="9" t="s">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J22" s="9"/>
+      <c r="J22" s="7"/>
     </row>
     <row r="23" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6" t="s">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
-      <c r="J24" s="6" t="s">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6" t="s">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="9" t="s">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J26" s="9"/>
+      <c r="J26" s="7"/>
     </row>
     <row r="27" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="6"/>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
-      <c r="J27" s="6" t="s">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6" t="s">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="6"/>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
-      <c r="J29" s="6" t="s">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2137,9 +2148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F179409-8CEA-4DDD-A3F6-CB10F00560A7}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2739,7 +2748,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2751,232 +2760,232 @@
       <c r="A1" t="s">
         <v>125</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AD1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AE1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AF1" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AG1" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AH1" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AI1" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AK1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AL1" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AM1" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AN1" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AO1" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AP1" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AQ1" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AR1" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AS1" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AT1" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AU1" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AV1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AW1" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AX1" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AY1" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="AZ1" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BA1" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BB1" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BC1" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BD1" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BE1" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BF1" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BG1" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BH1" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BI1" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BJ1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BK1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BL1" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BM1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BN1" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BO1" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BP1" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BQ1" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BR1" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BS1" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BT1" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BU1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="BV1" t="s">
+      <c r="BV1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="BW1" t="s">
+      <c r="BW1" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="BX1" t="s">
+      <c r="BX1" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="BY1" s="2" t="s">
+      <c r="BY1" s="6" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2984,237 +2993,237 @@
       <c r="A2" t="s">
         <v>32</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="5">
         <v>4</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="5">
         <v>5</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="5">
         <v>6</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="5">
         <v>7</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="5">
         <v>8</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="5">
         <v>9</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="5">
         <v>10</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="5">
         <v>11</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="5">
         <v>12</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="5">
         <v>13</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="5">
         <v>14</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="5">
         <v>15</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="5">
         <v>16</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="5">
         <v>17</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="5">
         <v>18</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="5">
         <v>19</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="5">
         <v>20</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="5">
         <v>21</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="5">
         <v>22</v>
       </c>
-      <c r="X2">
+      <c r="X2" s="5">
         <v>23</v>
       </c>
-      <c r="Y2">
+      <c r="Y2" s="5">
         <v>24</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="5">
         <v>25</v>
       </c>
-      <c r="AA2">
+      <c r="AA2" s="5">
         <v>26</v>
       </c>
-      <c r="AB2">
+      <c r="AB2" s="5">
         <v>27</v>
       </c>
-      <c r="AC2">
+      <c r="AC2" s="5">
         <v>28</v>
       </c>
-      <c r="AD2">
+      <c r="AD2" s="5">
         <v>29</v>
       </c>
-      <c r="AE2">
+      <c r="AE2" s="5">
         <v>30</v>
       </c>
-      <c r="AF2">
+      <c r="AF2" s="5">
         <v>31</v>
       </c>
-      <c r="AG2">
+      <c r="AG2" s="5">
         <v>32</v>
       </c>
-      <c r="AH2">
+      <c r="AH2" s="5">
         <v>33</v>
       </c>
-      <c r="AI2">
+      <c r="AI2" s="5">
         <v>34</v>
       </c>
-      <c r="AJ2">
+      <c r="AJ2" s="5">
         <v>35</v>
       </c>
-      <c r="AK2">
+      <c r="AK2" s="5">
         <v>36</v>
       </c>
-      <c r="AL2">
+      <c r="AL2" s="5">
         <v>37</v>
       </c>
-      <c r="AM2">
+      <c r="AM2" s="5">
         <v>38</v>
       </c>
-      <c r="AN2">
+      <c r="AN2" s="5">
         <v>39</v>
       </c>
-      <c r="AO2">
+      <c r="AO2" s="5">
         <v>40</v>
       </c>
-      <c r="AP2">
+      <c r="AP2" s="5">
         <v>41</v>
       </c>
-      <c r="AQ2">
+      <c r="AQ2" s="5">
         <v>42</v>
       </c>
-      <c r="AR2">
+      <c r="AR2" s="5">
         <v>43</v>
       </c>
-      <c r="AS2">
+      <c r="AS2" s="5">
         <v>44</v>
       </c>
-      <c r="AT2">
+      <c r="AT2" s="5">
         <v>45</v>
       </c>
-      <c r="AU2">
+      <c r="AU2" s="5">
         <v>46</v>
       </c>
-      <c r="AV2">
+      <c r="AV2" s="5">
         <v>47</v>
       </c>
-      <c r="AW2">
+      <c r="AW2" s="5">
         <v>48</v>
       </c>
-      <c r="AX2">
+      <c r="AX2" s="5">
         <v>49</v>
       </c>
-      <c r="AY2">
+      <c r="AY2" s="5">
         <v>50</v>
       </c>
-      <c r="AZ2">
+      <c r="AZ2" s="5">
         <v>51</v>
       </c>
-      <c r="BA2">
+      <c r="BA2" s="5">
         <v>52</v>
       </c>
-      <c r="BB2">
+      <c r="BB2" s="5">
         <v>53</v>
       </c>
-      <c r="BC2">
+      <c r="BC2" s="5">
         <v>54</v>
       </c>
-      <c r="BD2">
+      <c r="BD2" s="5">
         <v>55</v>
       </c>
-      <c r="BE2">
+      <c r="BE2" s="5">
         <v>56</v>
       </c>
-      <c r="BF2">
+      <c r="BF2" s="5">
         <v>57</v>
       </c>
-      <c r="BG2">
+      <c r="BG2" s="5">
         <v>58</v>
       </c>
-      <c r="BH2">
+      <c r="BH2" s="5">
         <v>59</v>
       </c>
-      <c r="BI2">
+      <c r="BI2" s="5">
         <v>60</v>
       </c>
-      <c r="BJ2">
+      <c r="BJ2" s="5">
         <v>61</v>
       </c>
-      <c r="BK2">
+      <c r="BK2" s="5">
         <v>62</v>
       </c>
-      <c r="BL2">
+      <c r="BL2" s="5">
         <v>63</v>
       </c>
-      <c r="BM2">
+      <c r="BM2" s="5">
         <v>64</v>
       </c>
-      <c r="BN2">
+      <c r="BN2" s="5">
         <v>65</v>
       </c>
-      <c r="BO2">
+      <c r="BO2" s="5">
         <v>66</v>
       </c>
-      <c r="BP2">
+      <c r="BP2" s="5">
         <v>67</v>
       </c>
-      <c r="BQ2">
+      <c r="BQ2" s="5">
         <v>68</v>
       </c>
-      <c r="BR2">
+      <c r="BR2" s="5">
         <v>69</v>
       </c>
-      <c r="BS2">
+      <c r="BS2" s="5">
         <v>70</v>
       </c>
-      <c r="BT2">
+      <c r="BT2" s="5">
         <v>71</v>
       </c>
-      <c r="BU2">
+      <c r="BU2" s="5">
         <v>72</v>
       </c>
-      <c r="BV2">
+      <c r="BV2" s="5">
         <v>73</v>
       </c>
-      <c r="BW2">
+      <c r="BW2" s="5">
         <v>74</v>
       </c>
-      <c r="BX2">
+      <c r="BX2" s="5">
         <v>75</v>
       </c>
-      <c r="BY2">
+      <c r="BY2" s="5">
         <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="5" t="s">
         <v>109</v>
       </c>
       <c r="B3">
@@ -3237,7 +3246,7 @@
       </c>
     </row>
     <row r="4" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>110</v>
       </c>
       <c r="B4">
@@ -3260,7 +3269,7 @@
       </c>
     </row>
     <row r="5" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>111</v>
       </c>
       <c r="B5">
@@ -3292,7 +3301,7 @@
       </c>
     </row>
     <row r="6" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>112</v>
       </c>
       <c r="B6">
@@ -3315,7 +3324,7 @@
       </c>
     </row>
     <row r="7" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="5" t="s">
         <v>113</v>
       </c>
       <c r="B7">
@@ -3338,7 +3347,7 @@
       </c>
     </row>
     <row r="8" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="5" t="s">
         <v>114</v>
       </c>
       <c r="B8">
@@ -3409,7 +3418,7 @@
       </c>
     </row>
     <row r="9" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="5" t="s">
         <v>115</v>
       </c>
       <c r="B9">
@@ -3480,7 +3489,7 @@
       </c>
     </row>
     <row r="10" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="5" t="s">
         <v>116</v>
       </c>
       <c r="B10">
@@ -3560,7 +3569,7 @@
       </c>
     </row>
     <row r="11" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="5" t="s">
         <v>117</v>
       </c>
       <c r="B11">
@@ -3640,7 +3649,7 @@
       </c>
     </row>
     <row r="12" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" s="5" t="s">
         <v>118</v>
       </c>
       <c r="B12">
@@ -3831,7 +3840,7 @@
       </c>
     </row>
     <row r="13" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>119</v>
       </c>
       <c r="B13">
@@ -4022,7 +4031,7 @@
       </c>
     </row>
     <row r="14" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" s="5" t="s">
         <v>120</v>
       </c>
       <c r="B14">
@@ -4189,7 +4198,7 @@
       </c>
     </row>
     <row r="15" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="A15" s="5" t="s">
         <v>121</v>
       </c>
       <c r="B15">
@@ -4356,7 +4365,7 @@
       </c>
     </row>
     <row r="16" spans="1:77" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" s="5" t="s">
         <v>122</v>
       </c>
       <c r="B16">
@@ -4523,7 +4532,7 @@
       </c>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" s="5" t="s">
         <v>123</v>
       </c>
       <c r="B17">
@@ -4537,7 +4546,7 @@
       </c>
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="A18" s="5" t="s">
         <v>124</v>
       </c>
       <c r="B18">

</xml_diff>